<commit_message>
Webservices trough TMAP in all project
</commit_message>
<xml_diff>
--- a/Antes de Iniciar/App Version Control.xlsx
+++ b/Antes de Iniciar/App Version Control.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Android Versions" sheetId="1" r:id="rId1"/>
     <sheet name="How To Set Android Versions" sheetId="2" r:id="rId2"/>
+    <sheet name="Previous RELEASE versions" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -84,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Major</t>
   </si>
@@ -294,6 +295,27 @@
   </si>
   <si>
     <t>dos para la versión del parche.</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>Versión</t>
+  </si>
+  <si>
+    <t>Cambios</t>
+  </si>
+  <si>
+    <t>Fecha del cambio</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>Cambios pedidos por Suarez Luis</t>
+  </si>
+  <si>
+    <t>Implementación TMAP en todo el proyecto</t>
   </si>
 </sst>
 </file>
@@ -390,7 +412,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,6 +440,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -525,6 +553,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1012,7 +1050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
@@ -2366,4 +2404,77 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="22.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="29">
+        <v>43404</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DELTA release WTT android app.(include APK)
</commit_message>
<xml_diff>
--- a/Antes de Iniciar/App Version Control.xlsx
+++ b/Antes de Iniciar/App Version Control.xlsx
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Major</t>
   </si>
@@ -316,6 +316,21 @@
   </si>
   <si>
     <t>Implementación TMAP en todo el proyecto</t>
+  </si>
+  <si>
+    <t>Issue 40629:Aplicación Task Mobile, issues varios</t>
+  </si>
+  <si>
+    <t>Mejora  visual en menú</t>
+  </si>
+  <si>
+    <t>Mejora visual en pantallas (tipografía,colores, símbolos de "pasos")</t>
+  </si>
+  <si>
+    <t>Agregado de la función "LOGOUT"/"CERRAR SESIÓN"</t>
+  </si>
+  <si>
+    <t>Almacenamiento Usuario en DB  y mostrar usuario desde DB en todas pantallas</t>
   </si>
 </sst>
 </file>
@@ -2408,17 +2423,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D8"/>
+  <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.42578125" style="1"/>
     <col min="3" max="3" width="22.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="71.7109375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -2461,17 +2476,37 @@
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
+      <c r="D6" s="28" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
+      <c r="D7" s="30" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
+      <c r="D8" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>